<commit_message>
with gigablocks. currently infeasible for the dummy values, check again
</commit_message>
<xml_diff>
--- a/preprocessing/MFMS_Daten_Dummy.xlsx
+++ b/preprocessing/MFMS_Daten_Dummy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theresawettig/superblock/preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ACFEDA-37FE-BA4C-B12B-968BDA376527}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FD05E4-330E-3C4B-B575-3B150DF28E4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="460" windowWidth="24440" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
   <si>
     <t>Center Typ</t>
   </si>
@@ -195,6 +195,15 @@
   </si>
   <si>
     <t>gigacenter</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>beta</t>
   </si>
 </sst>
 </file>
@@ -532,7 +541,7 @@
   <dimension ref="A1:H984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -543,7 +552,7 @@
     <col min="27" max="16384" width="12.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="16" t="s">
         <v>47</v>
       </c>
@@ -565,8 +574,11 @@
       <c r="G1" s="16" t="s">
         <v>52</v>
       </c>
+      <c r="H1" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -588,8 +600,11 @@
       <c r="G2" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="H2" s="6">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -611,8 +626,11 @@
       <c r="G3" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="H3" s="6">
+        <v>0.05</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -634,22 +652,50 @@
       <c r="G4" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="H4" s="6">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3000</v>
+      </c>
+      <c r="C5" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D5" s="6">
+        <v>250</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3000</v>
+      </c>
+      <c r="F5" s="6">
+        <v>20</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
     </row>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
     </row>

</xml_diff>

<commit_message>
constraint 6 was excluded for sb's that are already assigned; otherwise it would be infeasible
</commit_message>
<xml_diff>
--- a/preprocessing/MFMS_Daten_Dummy.xlsx
+++ b/preprocessing/MFMS_Daten_Dummy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theresawettig/superblock/preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FD05E4-330E-3C4B-B575-3B150DF28E4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815B81E0-1490-964A-8734-08EFF7F4FB21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="460" windowWidth="24440" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -541,7 +541,7 @@
   <dimension ref="A1:H984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -592,7 +592,7 @@
         <v>188.03418803418805</v>
       </c>
       <c r="E2" s="1">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="F2" s="1">
         <v>10</v>
@@ -618,7 +618,7 @@
         <v>900</v>
       </c>
       <c r="E3" s="1">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="F3" s="1">
         <v>70</v>
@@ -644,7 +644,7 @@
         <v>900</v>
       </c>
       <c r="E4" s="1">
-        <v>3000</v>
+        <v>8000</v>
       </c>
       <c r="F4" s="1">
         <v>20</v>
@@ -670,7 +670,7 @@
         <v>250</v>
       </c>
       <c r="E5" s="6">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="F5" s="6">
         <v>20</v>

</xml_diff>

<commit_message>
constraint 7 added (commercial buildings min. distance)
</commit_message>
<xml_diff>
--- a/preprocessing/MFMS_Daten_Dummy.xlsx
+++ b/preprocessing/MFMS_Daten_Dummy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theresawettig/superblock/preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A553091E-FC9C-A04A-B7A6-E3195B505D53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0810F369-FFBD-854E-A5EA-2F7EDFFEA27A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="480" windowWidth="24440" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3780" yWindow="3940" windowWidth="24440" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>Center Typ</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>beta</t>
+  </si>
+  <si>
+    <t>commercial</t>
   </si>
 </sst>
 </file>
@@ -538,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H984"/>
+  <dimension ref="A1:I984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -552,7 +555,7 @@
     <col min="27" max="16384" width="12.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="16" t="s">
         <v>47</v>
       </c>
@@ -577,22 +580,25 @@
       <c r="H1" s="6" t="s">
         <v>55</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>430</v>
+        <v>200</v>
       </c>
       <c r="C2" s="17">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="D2" s="1">
         <v>188.03418803418805</v>
       </c>
       <c r="E2" s="1">
-        <v>8000</v>
+        <v>50000</v>
       </c>
       <c r="F2" s="1">
         <v>10</v>
@@ -601,10 +607,13 @@
         <v>50</v>
       </c>
       <c r="H2" s="6">
-        <v>0.1</v>
+        <v>0.2</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -629,8 +638,11 @@
       <c r="H3" s="6">
         <v>0.05</v>
       </c>
+      <c r="I3" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -655,13 +667,16 @@
       <c r="H4" s="6">
         <v>0.1</v>
       </c>
+      <c r="I4" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="6">
-        <v>3000</v>
+        <v>13000</v>
       </c>
       <c r="C5" s="6">
         <v>5.0000000000000001E-3</v>
@@ -681,21 +696,24 @@
       <c r="H5" s="6">
         <v>0.1</v>
       </c>
+      <c r="I5" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
     </row>
-    <row r="16" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
     </row>

</xml_diff>

<commit_message>
#1 added constraint to consider superblock with gigacenters ( and no inhabitants) for getting the max. amount (upper bound) for placeable centers of a certain type
#2 constraitn to make sure that model isn't cheating with min. utilization by artifically increasing self visitors.
</commit_message>
<xml_diff>
--- a/preprocessing/MFMS_Daten_Dummy.xlsx
+++ b/preprocessing/MFMS_Daten_Dummy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theresawettig/superblock/preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0810F369-FFBD-854E-A5EA-2F7EDFFEA27A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB213FA8-CD2B-3C40-8572-4BDB8A103ED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="3940" windowWidth="24440" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="460" windowWidth="25500" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
   <dimension ref="A1:I984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E20" sqref="C7:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -665,7 +665,7 @@
         <v>50</v>
       </c>
       <c r="H4" s="6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>50</v>

</xml_diff>